<commit_message>
Historias de usuario aterrizadas previas al backlog
</commit_message>
<xml_diff>
--- a/Documentos/avances/Historias de usuarios.xlsx
+++ b/Documentos/avances/Historias de usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ISIL REDES Y COMUNICACIONES\Proyecto tecnologico\Proyecto-Tecnologico-2021-01-\Documentos\avances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E13BCE9-4B53-483A-B3B9-A352B6F87832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1DBD36-7D60-40D7-B774-A5875AEDC3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="138">
   <si>
     <t>Desarrollo ágil: Equipo 1 proyecto : Blondy's Siacca</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Al tener los productos de consumo interno y de venta separados, tenemor un mayor orden en el proceso de compra para la reposision de stock.</t>
   </si>
   <si>
-    <t>Blondys-005</t>
-  </si>
-  <si>
     <t>Necesito tener visibilidad de los cuartos ocupados y quien los ocupa.</t>
   </si>
   <si>
@@ -309,17 +306,152 @@
     <t xml:space="preserve">Al dar clic  en el recuadro redirecione de manera adecuada </t>
   </si>
   <si>
-    <t>RELEASE 1</t>
+    <t>Grado de importancia</t>
   </si>
   <si>
-    <t>Grado de importancia</t>
+    <t>Phone, Email, Website, Address</t>
+  </si>
+  <si>
+    <t>Muy importante</t>
+  </si>
+  <si>
+    <t>Importancia alta</t>
+  </si>
+  <si>
+    <t>Importancia media</t>
+  </si>
+  <si>
+    <t>Baja importancia</t>
+  </si>
+  <si>
+    <t>Mariella Pilar Lamonja Velasquez</t>
+  </si>
+  <si>
+    <t>mallelam08@gmail.com</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>¿Qué es importante para las partes interesadas?</t>
+  </si>
+  <si>
+    <t>¿Cómo podría contribuir la parte interesada al proyecto?</t>
+  </si>
+  <si>
+    <t>¿Cómo podría el interesado bloquear el proyecto?</t>
+  </si>
+  <si>
+    <t>Estrategia para involucrar a las partes interesadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre Stakeholder </t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Impacto</t>
+  </si>
+  <si>
+    <t>Influencia</t>
+  </si>
+  <si>
+    <t>¿Cuánto les afecta el proyecto?(Low, Medium, High)</t>
+  </si>
+  <si>
+    <t>¿Cuánta influencia tienen sobre el proyecto? (Low, Medium, High)</t>
+  </si>
+  <si>
+    <t>abel_dl@yahoo.es</t>
+  </si>
+  <si>
+    <t>Tener claridad sobre la satisfación de los clientes</t>
+  </si>
+  <si>
+    <t>Poder tener claridad sobre los clientes que ocupan habitación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explicando los procesos de negocio del día a día </t>
+  </si>
+  <si>
+    <t>Explicando la gestión con varias plataformas</t>
+  </si>
+  <si>
+    <t>Scrum Team</t>
+  </si>
+  <si>
+    <t>No brindando información</t>
+  </si>
+  <si>
+    <t>No retroalimentando el trabajo</t>
+  </si>
+  <si>
+    <t>No trabajando de manera adecuada</t>
+  </si>
+  <si>
+    <t>Desarrollar un buen proyecto</t>
+  </si>
+  <si>
+    <t>Mediante entrevistas</t>
+  </si>
+  <si>
+    <t>Demostración de sotfware</t>
+  </si>
+  <si>
+    <t>Dailys</t>
+  </si>
+  <si>
+    <t>trabajando conforme a lo pactado</t>
+  </si>
+  <si>
+    <t>Necesito poder crear usuarios</t>
+  </si>
+  <si>
+    <t>PRESENTACIÓN 1</t>
+  </si>
+  <si>
+    <t>Para poder tener un control sobre que tipo de acciones que pueden hacer o no en el sistema</t>
+  </si>
+  <si>
+    <t>Los usuarios creados  deben poder cumplir unicamente con los roles  asignados</t>
+  </si>
+  <si>
+    <t>Al crear al usuario debe solo poder cumplir , con los permisos que se le asigna</t>
+  </si>
+  <si>
+    <t>Por temas de crecimiento se planea contratar un personal solo para atender y debe contar con un usuario</t>
+  </si>
+  <si>
+    <t>El administrador pueda crear usuarios y otorgarles los permisos que necesita</t>
+  </si>
+  <si>
+    <t>Cargo</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Gerente general</t>
+  </si>
+  <si>
+    <t>Encargado de marketing</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abel Davila </t>
+  </si>
+  <si>
+    <t>Blondys-007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,8 +482,42 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,8 +572,44 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -664,11 +866,186 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -749,55 +1126,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,14 +1141,152 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1036,9 +1502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1046,14 +1512,16 @@
     <col min="1" max="1" width="1.453125" customWidth="1"/>
     <col min="2" max="2" width="13.6328125" style="27" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="23" style="27" customWidth="1"/>
+    <col min="4" max="4" width="26" style="27" customWidth="1"/>
+    <col min="5" max="5" width="105" style="27" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" style="27" customWidth="1"/>
     <col min="7" max="7" width="31.54296875" style="27" customWidth="1"/>
     <col min="8" max="8" width="35.6328125" style="27" customWidth="1"/>
     <col min="9" max="9" width="41.90625" style="27" customWidth="1"/>
     <col min="10" max="10" width="38.36328125" style="27" customWidth="1"/>
-    <col min="11" max="26" width="10" customWidth="1"/>
+    <col min="11" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="17.1796875" customWidth="1"/>
+    <col min="16" max="26" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="36" customHeight="1">
@@ -1100,8 +1568,12 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="63">
+        <v>1</v>
+      </c>
+      <c r="O2" s="64" t="s">
+        <v>93</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -1128,8 +1600,12 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="N3" s="65">
+        <v>2</v>
+      </c>
+      <c r="O3" s="66" t="s">
+        <v>94</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -1145,23 +1621,27 @@
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="53" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="N4" s="67">
+        <v>3</v>
+      </c>
+      <c r="O4" s="68" t="s">
+        <v>95</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -1203,13 +1683,17 @@
       <c r="J5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="51" t="s">
-        <v>93</v>
+      <c r="K5" s="30" t="s">
+        <v>91</v>
       </c>
-      <c r="L5" s="52"/>
+      <c r="L5" s="31"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="N5" s="69">
+        <v>4</v>
+      </c>
+      <c r="O5" s="70" t="s">
+        <v>96</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -1224,16 +1708,16 @@
     </row>
     <row r="6" spans="1:26" ht="130.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="35" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="6">
@@ -1251,10 +1735,10 @@
       <c r="J6" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="55">
+      <c r="K6" s="34">
         <v>1</v>
       </c>
-      <c r="L6" s="55"/>
+      <c r="L6" s="34"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1272,29 +1756,29 @@
     </row>
     <row r="7" spans="1:26" ht="28.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="43">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="35">
         <v>2</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="55">
+      <c r="K7" s="34">
         <v>3</v>
       </c>
-      <c r="L7" s="55"/>
+      <c r="L7" s="34"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1312,17 +1796,17 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1340,17 +1824,17 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="42"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1377,8 +1861,8 @@
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
-      <c r="K10" s="36"/>
-      <c r="L10" s="37"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="50"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1396,37 +1880,37 @@
     </row>
     <row r="11" spans="1:26" ht="28.5" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="35">
         <v>1</v>
       </c>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="41" t="s">
+      <c r="H11" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="41" t="s">
+      <c r="I11" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="55">
+      <c r="K11" s="34">
         <v>2</v>
       </c>
-      <c r="L11" s="55"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1444,17 +1928,17 @@
     </row>
     <row r="12" spans="1:26" ht="45" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1472,29 +1956,29 @@
     </row>
     <row r="13" spans="1:26" ht="28.25" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="43">
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="35">
         <v>2</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="41" t="s">
+      <c r="H13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="41" t="s">
+      <c r="I13" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="45" t="s">
+      <c r="J13" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="55">
+      <c r="K13" s="34">
         <v>1</v>
       </c>
-      <c r="L13" s="55"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1512,17 +1996,17 @@
     </row>
     <row r="14" spans="1:26" ht="42.75" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1549,8 +2033,8 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="52"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1568,7 +2052,7 @@
     </row>
     <row r="16" spans="1:26" ht="147.75" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="35" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
@@ -1595,10 +2079,10 @@
       <c r="J16" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="55">
+      <c r="K16" s="34">
         <v>3</v>
       </c>
-      <c r="L16" s="55"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1616,7 +2100,7 @@
     </row>
     <row r="17" spans="1:26" ht="92.25" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="42"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
@@ -1641,10 +2125,10 @@
       <c r="J17" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="55">
+      <c r="K17" s="34">
         <v>2</v>
       </c>
-      <c r="L17" s="55"/>
+      <c r="L17" s="34"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -1671,8 +2155,8 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="37"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="50"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1690,16 +2174,16 @@
     </row>
     <row r="19" spans="1:26" ht="58.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="35" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="14">
@@ -1717,10 +2201,10 @@
       <c r="J19" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="55">
+      <c r="K19" s="34">
         <v>3</v>
       </c>
-      <c r="L19" s="55"/>
+      <c r="L19" s="34"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1738,10 +2222,10 @@
     </row>
     <row r="20" spans="1:26" ht="80.25" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
       <c r="F20" s="14">
         <v>2</v>
       </c>
@@ -1757,8 +2241,8 @@
       <c r="J20" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1776,10 +2260,10 @@
     </row>
     <row r="21" spans="1:26" ht="75" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="14">
         <v>3</v>
       </c>
@@ -1795,8 +2279,8 @@
       <c r="J21" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
@@ -1823,8 +2307,8 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="28"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1842,37 +2326,37 @@
     </row>
     <row r="23" spans="1:26" ht="78.75" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="43" t="s">
+      <c r="E23" s="35" t="s">
         <v>67</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>68</v>
       </c>
       <c r="F23" s="14">
         <v>1</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H23" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="I23" s="7" t="s">
+      <c r="J23" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="J23" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" s="55">
+      <c r="K23" s="34">
         <v>3</v>
       </c>
-      <c r="L23" s="55"/>
+      <c r="L23" s="34"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1890,29 +2374,29 @@
     </row>
     <row r="24" spans="1:26" ht="60.75" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
       <c r="F24" s="6">
         <v>2</v>
       </c>
       <c r="G24" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="J24" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="K24" s="55">
+      <c r="K24" s="34">
         <v>2</v>
       </c>
-      <c r="L24" s="55"/>
+      <c r="L24" s="34"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1930,29 +2414,29 @@
     </row>
     <row r="25" spans="1:26" ht="66.75" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="6">
         <v>3</v>
       </c>
       <c r="G25" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="J25" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="J25" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="K25" s="55">
+      <c r="K25" s="34">
         <v>2</v>
       </c>
-      <c r="L25" s="55"/>
+      <c r="L25" s="34"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1998,37 +2482,37 @@
     </row>
     <row r="27" spans="1:26" ht="65.25" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="43" t="s">
+      <c r="E27" s="35" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>83</v>
       </c>
       <c r="F27" s="6">
         <v>1</v>
       </c>
       <c r="G27" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="I27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="J27" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="J27" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="K27" s="55">
+      <c r="K27" s="34">
         <v>4</v>
       </c>
-      <c r="L27" s="55"/>
+      <c r="L27" s="34"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -2046,29 +2530,29 @@
     </row>
     <row r="28" spans="1:26" ht="42.75" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="6">
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="7">
         <v>2</v>
       </c>
       <c r="G28" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="7" t="s">
+      <c r="I28" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="I28" s="7" t="s">
+      <c r="J28" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="J28" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="K28" s="55">
+      <c r="K28" s="34">
         <v>4</v>
       </c>
-      <c r="L28" s="55"/>
+      <c r="L28" s="34"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -2095,8 +2579,8 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="31"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="55"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -2112,119 +2596,81 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A30" s="1"/>
-      <c r="B30" s="38" t="s">
-        <v>92</v>
+    <row r="30" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A30"/>
+      <c r="B30" s="91" t="s">
+        <v>137</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A31" s="1"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A33" s="1"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+      <c r="C30" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="77">
+        <v>2</v>
+      </c>
+      <c r="G30" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="80" t="s">
+        <v>129</v>
+      </c>
+      <c r="I30" s="80" t="s">
+        <v>128</v>
+      </c>
+      <c r="J30" s="80" t="s">
+        <v>130</v>
+      </c>
+      <c r="K30" s="83">
+        <v>2</v>
+      </c>
+      <c r="L30" s="84"/>
+    </row>
+    <row r="31" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A31"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="81"/>
+      <c r="H31" s="81"/>
+      <c r="I31" s="81"/>
+      <c r="J31" s="81"/>
+      <c r="K31" s="85"/>
+      <c r="L31" s="86"/>
+    </row>
+    <row r="32" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A32"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="81"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="81"/>
+      <c r="J32" s="81"/>
+      <c r="K32" s="85"/>
+      <c r="L32" s="86"/>
+    </row>
+    <row r="33" spans="1:26" s="79" customFormat="1" ht="15" customHeight="1">
+      <c r="A33"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="88"/>
     </row>
     <row r="34" spans="1:26" ht="14.25" customHeight="1">
       <c r="A34" s="1"/>
@@ -2237,8 +2683,8 @@
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
-      <c r="K34" s="34"/>
-      <c r="L34" s="35"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -2256,17 +2702,19 @@
     </row>
     <row r="35" spans="1:26" ht="14.25" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
+      <c r="B35" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -2284,17 +2732,17 @@
     </row>
     <row r="36" spans="1:26" ht="14.25" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -2312,17 +2760,17 @@
     </row>
     <row r="37" spans="1:26" ht="14.25" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -2340,17 +2788,17 @@
     </row>
     <row r="38" spans="1:26" ht="14.25" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -2396,10 +2844,10 @@
     </row>
     <row r="40" spans="1:26" ht="14.25" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
       <c r="F40" s="20"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
@@ -2424,10 +2872,10 @@
     </row>
     <row r="41" spans="1:26" ht="14.25" customHeight="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="40"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="20"/>
       <c r="G41" s="21"/>
       <c r="H41" s="21"/>
@@ -2452,10 +2900,10 @@
     </row>
     <row r="42" spans="1:26" ht="14.25" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
       <c r="F42" s="20"/>
       <c r="G42" s="21"/>
       <c r="H42" s="21"/>
@@ -2480,10 +2928,10 @@
     </row>
     <row r="43" spans="1:26" ht="14.25" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
       <c r="F43" s="20"/>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
@@ -2536,10 +2984,10 @@
     </row>
     <row r="45" spans="1:26" ht="14.25" customHeight="1">
       <c r="A45" s="1"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
       <c r="F45" s="26"/>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
@@ -2564,10 +3012,10 @@
     </row>
     <row r="46" spans="1:26" ht="14.25" customHeight="1">
       <c r="A46" s="1"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
       <c r="F46" s="26"/>
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
@@ -2592,10 +3040,10 @@
     </row>
     <row r="47" spans="1:26" ht="14.25" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
       <c r="F47" s="26"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
@@ -2620,10 +3068,10 @@
     </row>
     <row r="48" spans="1:26" ht="14.25" customHeight="1">
       <c r="A48" s="1"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
       <c r="F48" s="26"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
@@ -2676,10 +3124,10 @@
     </row>
     <row r="50" spans="1:26" ht="14.25" customHeight="1">
       <c r="A50" s="1"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
       <c r="F50" s="26"/>
       <c r="G50" s="21"/>
       <c r="H50" s="21"/>
@@ -2704,10 +3152,10 @@
     </row>
     <row r="51" spans="1:26" ht="14.25" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
       <c r="F51" s="26"/>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
@@ -2732,10 +3180,10 @@
     </row>
     <row r="52" spans="1:26" ht="14.25" customHeight="1">
       <c r="A52" s="1"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="40"/>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
       <c r="F52" s="26"/>
       <c r="G52" s="21"/>
       <c r="H52" s="21"/>
@@ -2760,10 +3208,10 @@
     </row>
     <row r="53" spans="1:26" ht="14.25" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
       <c r="F53" s="26"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
@@ -2816,10 +3264,10 @@
     </row>
     <row r="55" spans="1:26" ht="14.25" customHeight="1">
       <c r="A55" s="1"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
+      <c r="B55" s="45"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
       <c r="F55" s="26"/>
       <c r="G55" s="21"/>
       <c r="H55" s="21"/>
@@ -2844,10 +3292,10 @@
     </row>
     <row r="56" spans="1:26" ht="14.25" customHeight="1">
       <c r="A56" s="1"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
       <c r="F56" s="26"/>
       <c r="G56" s="21"/>
       <c r="H56" s="21"/>
@@ -2872,10 +3320,10 @@
     </row>
     <row r="57" spans="1:26" ht="14.25" customHeight="1">
       <c r="A57" s="1"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="40"/>
-      <c r="E57" s="40"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
       <c r="F57" s="26"/>
       <c r="G57" s="21"/>
       <c r="H57" s="21"/>
@@ -2900,10 +3348,10 @@
     </row>
     <row r="58" spans="1:26" ht="14.25" customHeight="1">
       <c r="A58" s="1"/>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
       <c r="F58" s="26"/>
       <c r="G58" s="21"/>
       <c r="H58" s="21"/>
@@ -2956,10 +3404,10 @@
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1">
       <c r="A60" s="1"/>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
+      <c r="B60" s="45"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
       <c r="F60" s="26"/>
       <c r="G60" s="21"/>
       <c r="H60" s="21"/>
@@ -2984,10 +3432,10 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1">
       <c r="A61" s="1"/>
-      <c r="B61" s="40"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
       <c r="F61" s="26"/>
       <c r="G61" s="21"/>
       <c r="H61" s="21"/>
@@ -3012,10 +3460,10 @@
     </row>
     <row r="62" spans="1:26" ht="14.25" customHeight="1">
       <c r="A62" s="1"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
       <c r="F62" s="26"/>
       <c r="G62" s="21"/>
       <c r="H62" s="21"/>
@@ -3040,10 +3488,10 @@
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1">
       <c r="A63" s="1"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
       <c r="F63" s="26"/>
       <c r="G63" s="21"/>
       <c r="H63" s="21"/>
@@ -3096,10 +3544,10 @@
     </row>
     <row r="65" spans="1:26" ht="14.25" customHeight="1">
       <c r="A65" s="1"/>
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
       <c r="F65" s="26"/>
       <c r="G65" s="21"/>
       <c r="H65" s="21"/>
@@ -3124,10 +3572,10 @@
     </row>
     <row r="66" spans="1:26" ht="14.25" customHeight="1">
       <c r="A66" s="1"/>
-      <c r="B66" s="40"/>
-      <c r="C66" s="40"/>
-      <c r="D66" s="40"/>
-      <c r="E66" s="40"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="46"/>
       <c r="F66" s="26"/>
       <c r="G66" s="21"/>
       <c r="H66" s="21"/>
@@ -3152,10 +3600,10 @@
     </row>
     <row r="67" spans="1:26" ht="14.25" customHeight="1">
       <c r="A67" s="1"/>
-      <c r="B67" s="40"/>
-      <c r="C67" s="40"/>
-      <c r="D67" s="40"/>
-      <c r="E67" s="40"/>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
       <c r="F67" s="26"/>
       <c r="G67" s="21"/>
       <c r="H67" s="21"/>
@@ -3180,10 +3628,10 @@
     </row>
     <row r="68" spans="1:26" ht="14.25" customHeight="1">
       <c r="A68" s="1"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
       <c r="F68" s="26"/>
       <c r="G68" s="21"/>
       <c r="H68" s="21"/>
@@ -3236,10 +3684,10 @@
     </row>
     <row r="70" spans="1:26" ht="14.25" customHeight="1">
       <c r="A70" s="1"/>
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
+      <c r="B70" s="45"/>
+      <c r="C70" s="45"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
       <c r="F70" s="26"/>
       <c r="G70" s="21"/>
       <c r="H70" s="21"/>
@@ -3264,10 +3712,10 @@
     </row>
     <row r="71" spans="1:26" ht="14.25" customHeight="1">
       <c r="A71" s="1"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="40"/>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="46"/>
+      <c r="E71" s="46"/>
       <c r="F71" s="26"/>
       <c r="G71" s="21"/>
       <c r="H71" s="21"/>
@@ -3292,10 +3740,10 @@
     </row>
     <row r="72" spans="1:26" ht="14.25" customHeight="1">
       <c r="A72" s="1"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="40"/>
-      <c r="D72" s="40"/>
-      <c r="E72" s="40"/>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="46"/>
       <c r="F72" s="26"/>
       <c r="G72" s="21"/>
       <c r="H72" s="21"/>
@@ -3320,10 +3768,10 @@
     </row>
     <row r="73" spans="1:26" ht="14.25" customHeight="1">
       <c r="A73" s="1"/>
-      <c r="B73" s="40"/>
-      <c r="C73" s="40"/>
-      <c r="D73" s="40"/>
-      <c r="E73" s="40"/>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46"/>
+      <c r="D73" s="46"/>
+      <c r="E73" s="46"/>
       <c r="F73" s="26"/>
       <c r="G73" s="21"/>
       <c r="H73" s="21"/>
@@ -3376,10 +3824,10 @@
     </row>
     <row r="75" spans="1:26" ht="14.25" customHeight="1">
       <c r="A75" s="1"/>
-      <c r="B75" s="39"/>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
+      <c r="B75" s="45"/>
+      <c r="C75" s="45"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
       <c r="F75" s="26"/>
       <c r="G75" s="21"/>
       <c r="H75" s="21"/>
@@ -3404,10 +3852,10 @@
     </row>
     <row r="76" spans="1:26" ht="14.25" customHeight="1">
       <c r="A76" s="1"/>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
+      <c r="B76" s="46"/>
+      <c r="C76" s="46"/>
+      <c r="D76" s="46"/>
+      <c r="E76" s="46"/>
       <c r="F76" s="26"/>
       <c r="G76" s="21"/>
       <c r="H76" s="21"/>
@@ -3432,10 +3880,10 @@
     </row>
     <row r="77" spans="1:26" ht="14.25" customHeight="1">
       <c r="A77" s="1"/>
-      <c r="B77" s="40"/>
-      <c r="C77" s="40"/>
-      <c r="D77" s="40"/>
-      <c r="E77" s="40"/>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="46"/>
       <c r="F77" s="26"/>
       <c r="G77" s="21"/>
       <c r="H77" s="21"/>
@@ -3460,10 +3908,10 @@
     </row>
     <row r="78" spans="1:26" ht="14.25" customHeight="1">
       <c r="A78" s="1"/>
-      <c r="B78" s="40"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46"/>
+      <c r="D78" s="46"/>
+      <c r="E78" s="46"/>
       <c r="F78" s="26"/>
       <c r="G78" s="21"/>
       <c r="H78" s="21"/>
@@ -29134,20 +29582,81 @@
       <c r="Z994" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="97">
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E9"/>
-    <mergeCell ref="F7:F9"/>
+  <mergeCells count="103">
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="K30:L33"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="J30:J33"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="E30:E33"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K7:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="B35:L38"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="E60:E63"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="D65:D68"/>
+    <mergeCell ref="E65:E68"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="D70:D73"/>
+    <mergeCell ref="E70:E73"/>
+    <mergeCell ref="B70:B73"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="C50:C53"/>
+    <mergeCell ref="D50:D53"/>
+    <mergeCell ref="E50:E53"/>
+    <mergeCell ref="B50:B53"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="C55:C58"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D40:D43"/>
+    <mergeCell ref="E40:E43"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="F13:F14"/>
@@ -29164,74 +29673,19 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="C45:C48"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C50:C53"/>
-    <mergeCell ref="D50:D53"/>
-    <mergeCell ref="E50:E53"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="C55:C58"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="D40:D43"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="D65:D68"/>
-    <mergeCell ref="E65:E68"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="D70:D73"/>
-    <mergeCell ref="E70:E73"/>
-    <mergeCell ref="B70:B73"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K7:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="B30:L33"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -29240,17 +29694,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85C4751-40AE-40C2-8B4C-8DC62F391F83}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16384" width="11.54296875" style="27"/>
+    <col min="1" max="1" width="11.54296875" style="27"/>
+    <col min="2" max="2" width="28.36328125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.36328125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="21" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" style="27" customWidth="1"/>
+    <col min="7" max="7" width="52.6328125" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.90625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.54296875" style="27" customWidth="1"/>
+    <col min="10" max="10" width="23.54296875" style="27" customWidth="1"/>
+    <col min="11" max="16384" width="11.54296875" style="27"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:10" ht="14.5" customHeight="1">
+      <c r="B1" s="59" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="93" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="78" customHeight="1">
+      <c r="B2" s="75"/>
+      <c r="C2" s="92" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="72"/>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="J4" s="61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="61"/>
+      <c r="E5" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" s="61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{1E3C2CD8-7F93-468E-8F4B-90BADA69051D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>